<commit_message>
Wrote Test cases for Algorithm 2 to check specific value and their index
</commit_message>
<xml_diff>
--- a/Magic Square.xlsx
+++ b/Magic Square.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdulraziqadvani/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdulraziqadvani/Documents/Projects/Personal/magic-square-tdd-ts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8A374C-1F6B-244E-8A86-8277F3562E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540937BA-0E3A-E448-8694-541415F0F7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19100" activeTab="2" xr2:uid="{272B22AE-DA7E-3747-971D-0E13594C3976}"/>
   </bookViews>
   <sheets>
     <sheet name="3 x 3" sheetId="1" r:id="rId1"/>
-    <sheet name="5 x 5" sheetId="2" r:id="rId2"/>
-    <sheet name="7 x 7" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="5 x 5" sheetId="2" r:id="rId3"/>
+    <sheet name="7 x 7" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Number</t>
   </si>
@@ -72,13 +73,16 @@
   </si>
   <si>
     <t>1+1, 0-2</t>
+  </si>
+  <si>
+    <t>(5 * ((5^2) + 1)) / 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -99,16 +103,30 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -146,17 +164,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,269 +560,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4AC7B45-77ED-B143-B399-01E7EF1B2705}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="169" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A2" zoomScale="169" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="140" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="98" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="56" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507A5BA1-2838-0D4A-93C1-8224A11BF289}">
+  <dimension ref="B4:E11"/>
+  <sheetViews>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="4" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9">
+        <v>8</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <f>SUM(B5:D5)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9">
+        <v>5</v>
+      </c>
+      <c r="D6" s="10">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <f>SUM(B6:D6)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="C7" s="8">
         <v>9</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D7" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>4</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3284B31F-BC08-2A49-B354-E88E3DD9B172}">
-  <dimension ref="B3:F7"/>
-  <sheetViews>
-    <sheetView zoomScale="173" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="5">
-        <v>17</v>
-      </c>
-      <c r="C3" s="5">
-        <v>24</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5">
-        <v>8</v>
-      </c>
-      <c r="F3" s="5">
+      <c r="E7">
+        <f>SUM(B7:D7)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="5">
-        <v>23</v>
-      </c>
-      <c r="C4" s="5">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5">
-        <v>7</v>
-      </c>
-      <c r="E4" s="5">
-        <v>14</v>
-      </c>
-      <c r="F4" s="5">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5">
-        <v>13</v>
-      </c>
-      <c r="E5" s="5">
-        <v>20</v>
-      </c>
-      <c r="F5" s="5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="5">
-        <v>10</v>
-      </c>
-      <c r="C6" s="5">
+    <row r="8" spans="2:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f>SUM(B5:B7)</f>
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C5:C7)</f>
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <f>SUM(D5:D7)</f>
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <f>SUM(B5,C6,D7)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" s="5">
-        <v>19</v>
-      </c>
-      <c r="E6" s="5">
-        <v>21</v>
-      </c>
-      <c r="F6" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="5">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5">
-        <v>18</v>
-      </c>
-      <c r="D7" s="5">
-        <v>25</v>
-      </c>
-      <c r="E7" s="5">
-        <v>2</v>
-      </c>
-      <c r="F7" s="5">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -742,173 +819,274 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3284B31F-BC08-2A49-B354-E88E3DD9B172}">
+  <dimension ref="B3:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="G7" sqref="G3:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="4">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="4">
+        <v>23</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="4">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4">
+        <v>21</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="4">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4">
+        <v>25</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>9</v>
+      </c>
+      <c r="G7" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{572005A4-E5A2-6643-BBD4-E8D6268D0416}">
   <dimension ref="B3:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="211" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="211" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>30</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>39</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>48</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>1</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>10</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>19</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>38</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>47</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>7</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>9</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>18</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>27</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>46</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>6</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>8</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>17</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>26</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>35</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>5</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>14</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>16</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>25</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>34</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>36</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>13</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>15</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>24</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>33</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>42</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>44</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>21</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>23</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>32</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>41</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>43</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>3</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>22</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>31</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>40</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>49</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>2</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>11</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP: Wrote Magic Square Algorithm partial
</commit_message>
<xml_diff>
--- a/Magic Square.xlsx
+++ b/Magic Square.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdulraziqadvani/Documents/Projects/Personal/magic-square-tdd-ts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540937BA-0E3A-E448-8694-541415F0F7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C9076B-EE28-2741-ABFA-AAD90E92EC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19100" activeTab="2" xr2:uid="{272B22AE-DA7E-3747-971D-0E13594C3976}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{272B22AE-DA7E-3747-971D-0E13594C3976}"/>
   </bookViews>
   <sheets>
     <sheet name="3 x 3" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
-    <sheet name="5 x 5" sheetId="2" r:id="rId3"/>
-    <sheet name="7 x 7" sheetId="3" r:id="rId4"/>
+    <sheet name="5 x 5" sheetId="2" r:id="rId2"/>
+    <sheet name="7 x 7" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Number</t>
   </si>
@@ -73,9 +72,6 @@
   </si>
   <si>
     <t>1+1, 0-2</t>
-  </si>
-  <si>
-    <t>(5 * ((5^2) + 1)) / 2</t>
   </si>
 </sst>
 </file>
@@ -126,7 +122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -175,63 +171,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color theme="1"/>
-      </left>
-      <right style="thick">
-        <color theme="1"/>
-      </right>
-      <top style="thick">
-        <color theme="1"/>
-      </top>
-      <bottom style="thick">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="1"/>
-      </left>
-      <right style="thick">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color theme="1"/>
-      </right>
-      <top style="thick">
-        <color theme="1"/>
-      </top>
-      <bottom style="thick">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -241,11 +185,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4AC7B45-77ED-B143-B399-01E7EF1B2705}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="169" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="169" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,30 +512,30 @@
     <col min="1" max="1" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="140" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="140" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="98" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="98" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="56" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="56" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>8</v>
       </c>
@@ -605,7 +546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -616,7 +557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -626,9 +567,19 @@
       <c r="D8" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H8" s="8">
+        <f>1-1</f>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>0+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -636,7 +587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -650,7 +601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>1</v>
       </c>
@@ -661,7 +612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>2</v>
       </c>
@@ -675,7 +626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>3</v>
       </c>
@@ -689,7 +640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>4</v>
       </c>
@@ -703,29 +654,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>9</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -735,94 +716,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507A5BA1-2838-0D4A-93C1-8224A11BF289}">
-  <dimension ref="B4:E11"/>
-  <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="4" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
-        <v>8</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1</v>
-      </c>
-      <c r="D5" s="10">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <f>SUM(B5:D5)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
-        <v>3</v>
-      </c>
-      <c r="C6" s="9">
-        <v>5</v>
-      </c>
-      <c r="D6" s="10">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <f>SUM(B6:D6)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8">
-        <v>4</v>
-      </c>
-      <c r="C7" s="8">
-        <v>9</v>
-      </c>
-      <c r="D7" s="7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <f>SUM(B7:D7)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B8">
-        <f>SUM(B5:B7)</f>
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <f>SUM(C5:C7)</f>
-        <v>15</v>
-      </c>
-      <c r="D8">
-        <f>SUM(D5:D7)</f>
-        <v>15</v>
-      </c>
-      <c r="E8">
-        <f>SUM(B5,C6,D7)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3284B31F-BC08-2A49-B354-E88E3DD9B172}">
   <dimension ref="B3:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+    <sheetView zoomScale="173" workbookViewId="0">
       <selection activeCell="G7" sqref="G3:G7"/>
     </sheetView>
   </sheetViews>
@@ -912,14 +809,14 @@
       <c r="F7" s="4">
         <v>9</v>
       </c>
-      <c r="G7" s="11"/>
+      <c r="G7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{572005A4-E5A2-6643-BBD4-E8D6268D0416}">
   <dimension ref="B3:H9"/>
   <sheetViews>

</xml_diff>